<commit_message>
fix data kd 1-4
phân loại dữ liệu để phục vụ filter theo tags
</commit_message>
<xml_diff>
--- a/data/questions-data-test.xlsx
+++ b/data/questions-data-test.xlsx
@@ -7,7 +7,7 @@
     <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="TEST 20-12" sheetId="1" r:id="rId1"/>
     <sheet name="Hân" sheetId="2" r:id="rId2"/>
     <sheet name="BMC AN GIANG" sheetId="3" r:id="rId3"/>
     <sheet name="MY" sheetId="4" r:id="rId4"/>
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="274" uniqueCount="273">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="273" uniqueCount="272">
   <si>
     <t>name</t>
   </si>
@@ -522,9 +522,6 @@
   </si>
   <si>
     <t>Hiện nay xịt ốc bằng sản phẩm oosaka với liều 100g bình 25 lít, ruộng đủ nước nhưng ốc chết kém, chỉ khoảng 30%. Nguyên nhân tại sao?</t>
-  </si>
-  <si>
-    <t>answer</t>
   </si>
   <si>
     <t>bên cty em có sp nào, hoạt nào mát trị bọ trĩ, bọ xít muỗi, sâu, rầy, rệp , trị kiến ko?</t>
@@ -1218,12 +1215,18 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="2">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFF0000"/>
+        <bgColor indexed="64"/>
+      </patternFill>
     </fill>
   </fills>
   <borders count="1">
@@ -1238,7 +1241,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -1253,6 +1256,7 @@
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1533,108 +1537,103 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:C158"/>
+  <dimension ref="A1:B158"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A42" workbookViewId="0">
-      <selection activeCell="C58" sqref="C58"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B18" sqref="B18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="24.5703125" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="56.42578125" customWidth="1"/>
-    <col min="3" max="3" width="183" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
       <c r="B1" t="s">
         <v>1</v>
       </c>
-      <c r="C1" t="s">
-        <v>166</v>
-      </c>
-    </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>2</v>
       </c>
       <c r="B2" t="s">
         <v>3</v>
       </c>
-      <c r="C2" s="1"/>
-    </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
       <c r="B3" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
       <c r="B4" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="B5" t="s">
+    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="B5" s="6" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
       <c r="B6" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>8</v>
       </c>
-      <c r="B7" t="s">
+      <c r="B7" s="6" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:2" x14ac:dyDescent="0.25">
       <c r="B8" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="B9" t="s">
+    <row r="9" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="B9" s="6" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:2" x14ac:dyDescent="0.25">
       <c r="B10" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="11" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:2" x14ac:dyDescent="0.25">
       <c r="B11" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="12" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:2" x14ac:dyDescent="0.25">
       <c r="B12" t="s">
         <v>14</v>
       </c>
     </row>
-    <row r="13" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:2" x14ac:dyDescent="0.25">
       <c r="B13" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="14" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:2" x14ac:dyDescent="0.25">
       <c r="B14" t="s">
         <v>16</v>
       </c>
     </row>
-    <row r="15" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:2" x14ac:dyDescent="0.25">
       <c r="B15" t="s">
         <v>17</v>
       </c>
     </row>
-    <row r="16" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:2" x14ac:dyDescent="0.25">
       <c r="B16" t="s">
         <v>18</v>
       </c>
@@ -1798,7 +1797,7 @@
         <v>51</v>
       </c>
       <c r="B46" t="s">
-        <v>247</v>
+        <v>246</v>
       </c>
     </row>
     <row r="47" spans="1:2" x14ac:dyDescent="0.25">
@@ -2226,30 +2225,30 @@
     </row>
     <row r="125" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A125" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
       <c r="B125" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
     </row>
     <row r="126" spans="1:2" x14ac:dyDescent="0.25">
       <c r="B126" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
     </row>
     <row r="127" spans="1:2" x14ac:dyDescent="0.25">
       <c r="B127" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
     </row>
     <row r="128" spans="1:2" x14ac:dyDescent="0.25">
       <c r="B128" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
     </row>
     <row r="129" spans="1:2" x14ac:dyDescent="0.25">
       <c r="B129" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
     </row>
     <row r="130" spans="1:2" x14ac:dyDescent="0.25">
@@ -2377,30 +2376,30 @@
     </row>
     <row r="154" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A154" t="s">
+        <v>263</v>
+      </c>
+      <c r="B154" t="s">
         <v>264</v>
-      </c>
-      <c r="B154" t="s">
-        <v>265</v>
       </c>
     </row>
     <row r="155" spans="1:2" x14ac:dyDescent="0.25">
       <c r="B155" t="s">
-        <v>266</v>
+        <v>265</v>
       </c>
     </row>
     <row r="156" spans="1:2" x14ac:dyDescent="0.25">
       <c r="B156" t="s">
-        <v>267</v>
+        <v>266</v>
       </c>
     </row>
     <row r="157" spans="1:2" x14ac:dyDescent="0.25">
       <c r="B157" t="s">
-        <v>268</v>
+        <v>267</v>
       </c>
     </row>
     <row r="158" spans="1:2" x14ac:dyDescent="0.25">
       <c r="B158" t="s">
-        <v>269</v>
+        <v>268</v>
       </c>
     </row>
   </sheetData>
@@ -2425,42 +2424,42 @@
   <sheetData>
     <row r="1" spans="1:2" ht="75" x14ac:dyDescent="0.25">
       <c r="A1" s="2" t="s">
+        <v>172</v>
+      </c>
+      <c r="B1" s="2" t="s">
         <v>173</v>
-      </c>
-      <c r="B1" s="2" t="s">
-        <v>174</v>
       </c>
     </row>
     <row r="2" spans="1:2" ht="255" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
+        <v>174</v>
+      </c>
+      <c r="B2" s="2" t="s">
         <v>175</v>
-      </c>
-      <c r="B2" s="2" t="s">
-        <v>176</v>
       </c>
     </row>
     <row r="3" spans="1:2" ht="120" x14ac:dyDescent="0.25">
       <c r="A3" s="2" t="s">
+        <v>176</v>
+      </c>
+      <c r="B3" s="2" t="s">
         <v>177</v>
-      </c>
-      <c r="B3" s="2" t="s">
-        <v>178</v>
       </c>
     </row>
     <row r="4" spans="1:2" ht="120" x14ac:dyDescent="0.25">
       <c r="A4" s="2" t="s">
+        <v>178</v>
+      </c>
+      <c r="B4" s="2" t="s">
         <v>179</v>
-      </c>
-      <c r="B4" s="2" t="s">
-        <v>180</v>
       </c>
     </row>
     <row r="5" spans="1:2" ht="255" x14ac:dyDescent="0.25">
       <c r="A5" s="2" t="s">
+        <v>180</v>
+      </c>
+      <c r="B5" s="2" t="s">
         <v>181</v>
-      </c>
-      <c r="B5" s="2" t="s">
-        <v>182</v>
       </c>
     </row>
   </sheetData>
@@ -2484,218 +2483,218 @@
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
-        <v>183</v>
+        <v>182</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>185</v>
+        <v>184</v>
       </c>
     </row>
     <row r="2" spans="1:2" ht="135" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
-        <v>184</v>
+        <v>183</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>186</v>
+        <v>185</v>
       </c>
     </row>
     <row r="3" spans="1:2" ht="210" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
+        <v>186</v>
+      </c>
+      <c r="B3" s="1" t="s">
         <v>187</v>
-      </c>
-      <c r="B3" s="1" t="s">
-        <v>188</v>
       </c>
     </row>
     <row r="4" spans="1:2" ht="90" x14ac:dyDescent="0.25">
       <c r="A4" s="1" t="s">
+        <v>188</v>
+      </c>
+      <c r="B4" s="1" t="s">
         <v>189</v>
-      </c>
-      <c r="B4" s="1" t="s">
-        <v>190</v>
       </c>
     </row>
     <row r="5" spans="1:2" ht="240" x14ac:dyDescent="0.25">
       <c r="A5" s="1" t="s">
+        <v>190</v>
+      </c>
+      <c r="B5" s="1" t="s">
         <v>191</v>
-      </c>
-      <c r="B5" s="1" t="s">
-        <v>192</v>
       </c>
     </row>
     <row r="6" spans="1:2" ht="409.5" x14ac:dyDescent="0.25">
       <c r="A6" s="1" t="s">
+        <v>192</v>
+      </c>
+      <c r="B6" s="1" t="s">
         <v>193</v>
-      </c>
-      <c r="B6" s="1" t="s">
-        <v>194</v>
       </c>
     </row>
     <row r="7" spans="1:2" ht="285" x14ac:dyDescent="0.25">
       <c r="A7" s="1" t="s">
+        <v>194</v>
+      </c>
+      <c r="B7" s="1" t="s">
         <v>195</v>
-      </c>
-      <c r="B7" s="1" t="s">
-        <v>196</v>
       </c>
     </row>
     <row r="8" spans="1:2" ht="165" x14ac:dyDescent="0.25">
       <c r="A8" s="1" t="s">
+        <v>196</v>
+      </c>
+      <c r="B8" s="1" t="s">
         <v>197</v>
-      </c>
-      <c r="B8" s="1" t="s">
-        <v>198</v>
       </c>
     </row>
     <row r="9" spans="1:2" ht="150" x14ac:dyDescent="0.25">
       <c r="A9" s="1" t="s">
-        <v>199</v>
+        <v>198</v>
       </c>
       <c r="B9" s="1" t="s">
-        <v>257</v>
+        <v>256</v>
       </c>
     </row>
     <row r="10" spans="1:2" ht="195" x14ac:dyDescent="0.25">
       <c r="A10" s="1" t="s">
-        <v>200</v>
+        <v>199</v>
       </c>
       <c r="B10" s="1" t="s">
-        <v>258</v>
+        <v>257</v>
       </c>
     </row>
     <row r="11" spans="1:2" ht="60" x14ac:dyDescent="0.25">
       <c r="A11" s="1" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
       <c r="B11" s="1" t="s">
-        <v>259</v>
+        <v>258</v>
       </c>
     </row>
     <row r="12" spans="1:2" ht="30" x14ac:dyDescent="0.25">
       <c r="A12" s="1" t="s">
+        <v>201</v>
+      </c>
+      <c r="B12" s="3" t="s">
         <v>202</v>
-      </c>
-      <c r="B12" s="3" t="s">
-        <v>203</v>
       </c>
     </row>
     <row r="13" spans="1:2" ht="165" x14ac:dyDescent="0.25">
       <c r="A13" s="1" t="s">
+        <v>203</v>
+      </c>
+      <c r="B13" s="1" t="s">
         <v>204</v>
-      </c>
-      <c r="B13" s="1" t="s">
-        <v>205</v>
       </c>
     </row>
     <row r="14" spans="1:2" ht="60" x14ac:dyDescent="0.25">
       <c r="A14" s="1" t="s">
+        <v>205</v>
+      </c>
+      <c r="B14" s="1" t="s">
         <v>206</v>
-      </c>
-      <c r="B14" s="1" t="s">
-        <v>207</v>
       </c>
     </row>
     <row r="15" spans="1:2" ht="45" x14ac:dyDescent="0.25">
       <c r="A15" s="1" t="s">
+        <v>207</v>
+      </c>
+      <c r="B15" s="1" t="s">
         <v>208</v>
-      </c>
-      <c r="B15" s="1" t="s">
-        <v>209</v>
       </c>
     </row>
     <row r="16" spans="1:2" ht="120" x14ac:dyDescent="0.25">
       <c r="A16" s="1" t="s">
-        <v>210</v>
+        <v>209</v>
       </c>
       <c r="B16" s="1" t="s">
-        <v>254</v>
+        <v>253</v>
       </c>
     </row>
     <row r="17" spans="1:2" ht="210" x14ac:dyDescent="0.25">
       <c r="A17" s="4" t="s">
-        <v>212</v>
+        <v>211</v>
       </c>
       <c r="B17" s="4" t="s">
-        <v>256</v>
+        <v>255</v>
       </c>
     </row>
     <row r="18" spans="1:2" ht="360" x14ac:dyDescent="0.25">
       <c r="A18" s="1" t="s">
+        <v>212</v>
+      </c>
+      <c r="B18" s="1" t="s">
         <v>213</v>
-      </c>
-      <c r="B18" s="1" t="s">
-        <v>214</v>
       </c>
     </row>
     <row r="19" spans="1:2" ht="120" x14ac:dyDescent="0.25">
       <c r="A19" s="1" t="s">
+        <v>214</v>
+      </c>
+      <c r="B19" s="1" t="s">
         <v>215</v>
-      </c>
-      <c r="B19" s="1" t="s">
-        <v>216</v>
       </c>
     </row>
     <row r="20" spans="1:2" ht="60" x14ac:dyDescent="0.25">
       <c r="A20" s="1" t="s">
+        <v>216</v>
+      </c>
+      <c r="B20" s="1" t="s">
         <v>217</v>
-      </c>
-      <c r="B20" s="1" t="s">
-        <v>218</v>
       </c>
     </row>
     <row r="21" spans="1:2" ht="150" x14ac:dyDescent="0.25">
       <c r="A21" s="1" t="s">
+        <v>218</v>
+      </c>
+      <c r="B21" s="1" t="s">
         <v>219</v>
-      </c>
-      <c r="B21" s="1" t="s">
-        <v>220</v>
       </c>
     </row>
     <row r="22" spans="1:2" ht="75" x14ac:dyDescent="0.25">
       <c r="A22" s="1" t="s">
+        <v>220</v>
+      </c>
+      <c r="B22" s="1" t="s">
         <v>221</v>
-      </c>
-      <c r="B22" s="1" t="s">
-        <v>222</v>
       </c>
     </row>
     <row r="23" spans="1:2" ht="285" x14ac:dyDescent="0.25">
       <c r="A23" s="1" t="s">
+        <v>222</v>
+      </c>
+      <c r="B23" s="1" t="s">
         <v>223</v>
-      </c>
-      <c r="B23" s="1" t="s">
-        <v>224</v>
       </c>
     </row>
     <row r="24" spans="1:2" ht="120" x14ac:dyDescent="0.25">
       <c r="A24" s="1" t="s">
-        <v>225</v>
+        <v>224</v>
       </c>
       <c r="B24" s="1" t="s">
-        <v>255</v>
+        <v>254</v>
       </c>
     </row>
     <row r="25" spans="1:2" ht="285" x14ac:dyDescent="0.25">
       <c r="A25" s="1" t="s">
+        <v>225</v>
+      </c>
+      <c r="B25" s="1" t="s">
         <v>226</v>
-      </c>
-      <c r="B25" s="1" t="s">
-        <v>227</v>
       </c>
     </row>
     <row r="26" spans="1:2" ht="375" x14ac:dyDescent="0.25">
       <c r="A26" s="4" t="s">
-        <v>228</v>
+        <v>227</v>
       </c>
       <c r="B26" s="4" t="s">
-        <v>260</v>
+        <v>259</v>
       </c>
     </row>
     <row r="27" spans="1:2" ht="75" x14ac:dyDescent="0.25">
       <c r="A27" s="1" t="s">
+        <v>228</v>
+      </c>
+      <c r="B27" s="1" t="s">
         <v>229</v>
-      </c>
-      <c r="B27" s="1" t="s">
-        <v>230</v>
       </c>
     </row>
   </sheetData>
@@ -2719,42 +2718,42 @@
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>231</v>
+        <v>230</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>211</v>
+        <v>210</v>
       </c>
     </row>
     <row r="2" spans="1:2" ht="240" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
+        <v>231</v>
+      </c>
+      <c r="B2" s="1" t="s">
         <v>232</v>
-      </c>
-      <c r="B2" s="1" t="s">
-        <v>233</v>
       </c>
     </row>
     <row r="3" spans="1:2" ht="135" x14ac:dyDescent="0.25">
       <c r="A3" s="5" t="s">
-        <v>234</v>
+        <v>233</v>
       </c>
       <c r="B3" s="4" t="s">
-        <v>261</v>
+        <v>260</v>
       </c>
     </row>
     <row r="4" spans="1:2" ht="105" x14ac:dyDescent="0.25">
       <c r="A4" s="5" t="s">
-        <v>235</v>
+        <v>234</v>
       </c>
       <c r="B4" s="4" t="s">
-        <v>262</v>
+        <v>261</v>
       </c>
     </row>
     <row r="5" spans="1:2" ht="150" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
+        <v>235</v>
+      </c>
+      <c r="B5" s="1" t="s">
         <v>236</v>
-      </c>
-      <c r="B5" s="1" t="s">
-        <v>237</v>
       </c>
     </row>
   </sheetData>
@@ -2778,42 +2777,42 @@
   <sheetData>
     <row r="1" spans="1:2" ht="60" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>238</v>
+        <v>237</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>240</v>
+        <v>239</v>
       </c>
     </row>
     <row r="2" spans="1:2" ht="90" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>239</v>
+        <v>238</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>263</v>
+        <v>262</v>
       </c>
     </row>
     <row r="3" spans="1:2" ht="409.5" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
+        <v>240</v>
+      </c>
+      <c r="B3" s="3" t="s">
         <v>241</v>
-      </c>
-      <c r="B3" s="3" t="s">
-        <v>242</v>
       </c>
     </row>
     <row r="4" spans="1:2" ht="315" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
+        <v>242</v>
+      </c>
+      <c r="B4" s="1" t="s">
         <v>243</v>
-      </c>
-      <c r="B4" s="1" t="s">
-        <v>244</v>
       </c>
     </row>
     <row r="5" spans="1:2" ht="105" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
+        <v>244</v>
+      </c>
+      <c r="B5" s="1" t="s">
         <v>245</v>
-      </c>
-      <c r="B5" s="1" t="s">
-        <v>246</v>
       </c>
     </row>
   </sheetData>
@@ -2837,34 +2836,34 @@
   <sheetData>
     <row r="1" spans="1:2" ht="75" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
-        <v>248</v>
+        <v>247</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>270</v>
+        <v>269</v>
       </c>
     </row>
     <row r="2" spans="1:2" ht="180" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
-        <v>249</v>
+        <v>248</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>271</v>
+        <v>270</v>
       </c>
     </row>
     <row r="3" spans="1:2" ht="135" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
+        <v>249</v>
+      </c>
+      <c r="B3" s="1" t="s">
         <v>250</v>
-      </c>
-      <c r="B3" s="1" t="s">
-        <v>251</v>
       </c>
     </row>
     <row r="4" spans="1:2" ht="210" x14ac:dyDescent="0.25">
       <c r="A4" s="1" t="s">
-        <v>252</v>
+        <v>251</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>272</v>
+        <v>271</v>
       </c>
     </row>
     <row r="5" spans="1:2" ht="120" x14ac:dyDescent="0.25">
@@ -2872,7 +2871,7 @@
         <v>55</v>
       </c>
       <c r="B5" s="1" t="s">
-        <v>253</v>
+        <v>252</v>
       </c>
     </row>
   </sheetData>

</xml_diff>